<commit_message>
added lightgbm model results
</commit_message>
<xml_diff>
--- a/2021_04_11_Final/model_results.xlsx
+++ b/2021_04_11_Final/model_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\Python_Scripts\class\UCB\207\w207_final_project_bwp\0_experiments\kevin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinpi\MIDS\w207_final_project_bwp\2021_04_11_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38237399-E50A-490F-9160-73C494D4F788}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE86633-A1E1-45A5-91FF-17217F7B057B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5805" windowWidth="21840" windowHeight="13740" xr2:uid="{8502571B-A512-41BA-B560-0A8CC948E526}"/>
+    <workbookView xWindow="1716" yWindow="1260" windowWidth="15516" windowHeight="9882" xr2:uid="{8502571B-A512-41BA-B560-0A8CC948E526}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t>model</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>k_acc</t>
+  </si>
+  <si>
+    <t>LightGBM</t>
   </si>
 </sst>
 </file>
@@ -151,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -161,14 +164,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -191,6 +199,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="right" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -266,8 +275,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB8B7FB5-9E5C-449A-9DF4-D8002EB616B4}" name="Table1" displayName="Table1" ref="A1:E17" totalsRowShown="0">
-  <autoFilter ref="A1:E17" xr:uid="{636AB197-3477-4F2E-928C-C8C729D594CA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB8B7FB5-9E5C-449A-9DF4-D8002EB616B4}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0">
+  <autoFilter ref="A1:E21" xr:uid="{636AB197-3477-4F2E-928C-C8C729D594CA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{AED51CB8-0917-4809-B2CA-C34ED9FCFD19}" name="version" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{2400B6BF-1B0B-4F18-91E0-13CEA235E806}" name="model" dataDxfId="3"/>
@@ -576,26 +585,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5706A91-70A0-4CE1-B2FA-D535CC2E1280}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.68359375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.83984375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.83984375" customWidth="1"/>
+    <col min="4" max="4" width="18.83984375" customWidth="1"/>
+    <col min="5" max="5" width="15.41796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
@@ -604,7 +613,7 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="1"/>
@@ -614,10 +623,10 @@
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="9">
+      <c r="A2" s="7">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4">
@@ -626,16 +635,16 @@
       <c r="D2" s="4">
         <v>5.99198269844055</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="10">
         <v>0.75734999999999997</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4">
@@ -644,16 +653,16 @@
       <c r="D3" s="4">
         <v>48.949499368667603</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="10">
         <v>0.75934000000000001</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4">
@@ -662,16 +671,16 @@
       <c r="D4" s="4">
         <v>6.4758136272430402</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="11">
         <v>0.75431999999999999</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>0</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4">
@@ -680,230 +689,301 @@
       <c r="D5" s="4">
         <v>77.387502193450899</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="10">
         <v>0.73890999999999996</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.87239999999999995</v>
+      </c>
+      <c r="D6" s="4">
+        <v>56.443899999999999</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.75253999999999999</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7">
         <v>1</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C7" s="4">
         <v>0.89093915343915298</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="4">
         <v>5.7862265110015798</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E7" s="10">
         <v>0.79727000000000003</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="9">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="7">
         <v>1</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8" s="4">
         <v>0.892989417989418</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8" s="4">
         <v>45.508501768112097</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E8" s="10">
         <v>0.79788999999999999</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="9">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="7">
         <v>1</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C9" s="4">
         <v>0.88148148148148098</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9" s="4">
         <v>6.1565680503845197</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E9" s="10">
         <v>0.78393000000000002</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="9">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C10" s="4">
         <v>0.86216931216931203</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="4">
         <v>82.544497728347693</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="10">
         <v>0.74616000000000005</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="9">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="7">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.88090000000000002</v>
+      </c>
+      <c r="D11" s="4">
+        <v>64.006299999999996</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.76978000000000002</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="7">
         <v>2</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C12" s="4">
         <v>0.896560846560846</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D12" s="4">
         <v>5.6229577064514098</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E12" s="10">
         <v>0.80054999999999998</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="9">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="7">
         <v>2</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C13" s="4">
         <v>0.89755291005290905</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D13" s="4">
         <v>45.323498725891099</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E13" s="10">
         <v>0.80125000000000002</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="9">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="7">
         <v>2</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C14" s="4">
         <v>0.88029100529100501</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D14" s="4">
         <v>6.1019423007964999</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E14" s="10">
         <v>0.77829999999999999</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="9">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="7">
         <v>2</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C15" s="4">
         <v>0.862896825396825</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D15" s="4">
         <v>82.433997392654405</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E15" s="10">
         <v>0.75097999999999998</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="9">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="7">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.8821</v>
+      </c>
+      <c r="D16" s="4">
+        <v>64.049199999999999</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.77070000000000005</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="7">
         <v>3</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C17" s="4">
         <v>0.91111111111111098</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D17" s="4">
         <v>5.18176221847534</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E17" s="10">
         <v>0.81398999999999999</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="9">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="7">
         <v>3</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C18" s="4">
         <v>0.91309523809523796</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D18" s="4">
         <v>45.2369995117187</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E18" s="10">
         <v>0.81652999999999998</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="9">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="7">
         <v>3</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C19" s="4">
         <v>0.89318783068783003</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D19" s="4">
         <v>6.8079984188079798</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E19" s="11">
         <v>0.78535999999999995</v>
       </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="9">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="7">
         <v>3</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C20" s="4">
         <v>0.87559523809523798</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D20" s="4">
         <v>96.338500499725299</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E20" s="10">
         <v>0.75775999999999999</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" ht="13.8" customHeight="1">
+      <c r="A21" s="7">
+        <v>3</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.89670000000000005</v>
+      </c>
+      <c r="D21" s="4">
+        <v>72.608500000000006</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.78551000000000004</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
updated intro, added XGB and NN models, misc bug fixes to stitch code
</commit_message>
<xml_diff>
--- a/2021_04_11_Final/model_results.xlsx
+++ b/2021_04_11_Final/model_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinpi\MIDS\w207_final_project_bwp\2021_04_11_Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blairjones/Dropbox/-GradSchool/BerkeleyProgram/Semester2/W207-MachineLearning/w207_final_project_bwp/2021_04_11_Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE86633-A1E1-45A5-91FF-17217F7B057B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609B029E-3D72-6442-8A7F-D63CA7FD6FDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1716" yWindow="1260" windowWidth="15516" windowHeight="9882" xr2:uid="{8502571B-A512-41BA-B560-0A8CC948E526}"/>
+    <workbookView xWindow="1720" yWindow="1260" windowWidth="23140" windowHeight="13400" xr2:uid="{8502571B-A512-41BA-B560-0A8CC948E526}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>model</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>LightGBM</t>
+  </si>
+  <si>
+    <t>XGBoost</t>
+  </si>
+  <si>
+    <t>NeuralNetwork</t>
   </si>
 </sst>
 </file>
@@ -275,8 +281,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB8B7FB5-9E5C-449A-9DF4-D8002EB616B4}" name="Table1" displayName="Table1" ref="A1:E21" totalsRowShown="0">
-  <autoFilter ref="A1:E21" xr:uid="{636AB197-3477-4F2E-928C-C8C729D594CA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EB8B7FB5-9E5C-449A-9DF4-D8002EB616B4}" name="Table1" displayName="Table1" ref="A1:E29" totalsRowShown="0">
+  <autoFilter ref="A1:E29" xr:uid="{636AB197-3477-4F2E-928C-C8C729D594CA}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{AED51CB8-0917-4809-B2CA-C34ED9FCFD19}" name="version" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{2400B6BF-1B0B-4F18-91E0-13CEA235E806}" name="model" dataDxfId="3"/>
@@ -585,19 +591,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5706A91-70A0-4CE1-B2FA-D535CC2E1280}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.68359375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="20.83984375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15.83984375" customWidth="1"/>
-    <col min="4" max="4" width="18.83984375" customWidth="1"/>
-    <col min="5" max="5" width="15.41796875" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -681,16 +687,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4">
-        <v>0.85939153439153404</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="D5" s="4">
-        <v>77.387502193450899</v>
-      </c>
-      <c r="E5" s="10">
-        <v>0.73890999999999996</v>
+        <v>16.648</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.79200000000000004</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -699,52 +705,52 @@
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4">
-        <v>0.87239999999999995</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="D6" s="4">
-        <v>56.443899999999999</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0.75253999999999999</v>
+        <v>78.917199999999994</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.83099999999999996</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C7" s="4">
-        <v>0.89093915343915298</v>
+        <v>0.85939153439153404</v>
       </c>
       <c r="D7" s="4">
-        <v>5.7862265110015798</v>
+        <v>77.387502193450899</v>
       </c>
       <c r="E7" s="10">
-        <v>0.79727000000000003</v>
+        <v>0.73890999999999996</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4">
-        <v>0.892989417989418</v>
+        <v>0.87239999999999995</v>
       </c>
       <c r="D8" s="4">
-        <v>45.508501768112097</v>
+        <v>56.443899999999999</v>
       </c>
       <c r="E8" s="10">
-        <v>0.79788999999999999</v>
+        <v>0.75253999999999999</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -753,16 +759,16 @@
         <v>1</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="4">
-        <v>0.88148148148148098</v>
+        <v>0.89093915343915298</v>
       </c>
       <c r="D9" s="4">
-        <v>6.1565680503845197</v>
+        <v>5.7862265110015798</v>
       </c>
       <c r="E9" s="10">
-        <v>0.78393000000000002</v>
+        <v>0.79727000000000003</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -771,16 +777,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C10" s="4">
-        <v>0.86216931216931203</v>
+        <v>0.892989417989418</v>
       </c>
       <c r="D10" s="4">
-        <v>82.544497728347693</v>
+        <v>45.508501768112097</v>
       </c>
       <c r="E10" s="10">
-        <v>0.74616000000000005</v>
+        <v>0.79788999999999999</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -789,88 +795,88 @@
         <v>1</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" s="4">
-        <v>0.88090000000000002</v>
+        <v>0.88148148148148098</v>
       </c>
       <c r="D11" s="4">
-        <v>64.006299999999996</v>
+        <v>6.1565680503845197</v>
       </c>
       <c r="E11" s="10">
-        <v>0.76978000000000002</v>
+        <v>0.78393000000000002</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4">
-        <v>0.896560846560846</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="D12" s="4">
-        <v>5.6229577064514098</v>
+        <v>24.084299999999999</v>
       </c>
       <c r="E12" s="10">
-        <v>0.80054999999999998</v>
+        <v>0.81</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4">
-        <v>0.89755291005290905</v>
+        <v>0.95299999999999996</v>
       </c>
       <c r="D13" s="4">
-        <v>45.323498725891099</v>
+        <v>88.8048</v>
       </c>
       <c r="E13" s="10">
-        <v>0.80125000000000002</v>
+        <v>0.84099999999999997</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="4">
-        <v>0.88029100529100501</v>
+        <v>0.86216931216931203</v>
       </c>
       <c r="D14" s="4">
-        <v>6.1019423007964999</v>
+        <v>82.544497728347693</v>
       </c>
       <c r="E14" s="10">
-        <v>0.77829999999999999</v>
+        <v>0.74616000000000005</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C15" s="4">
-        <v>0.862896825396825</v>
+        <v>0.88090000000000002</v>
       </c>
       <c r="D15" s="4">
-        <v>82.433997392654405</v>
+        <v>64.006299999999996</v>
       </c>
       <c r="E15" s="10">
-        <v>0.75097999999999998</v>
+        <v>0.76978000000000002</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -879,105 +885,249 @@
         <v>2</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4">
-        <v>0.8821</v>
+        <v>0.896560846560846</v>
       </c>
       <c r="D16" s="4">
-        <v>64.049199999999999</v>
+        <v>5.6229577064514098</v>
       </c>
       <c r="E16" s="10">
-        <v>0.77070000000000005</v>
+        <v>0.80054999999999998</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="7">
+        <v>2</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>1</v>
-      </c>
       <c r="C17" s="4">
-        <v>0.91111111111111098</v>
+        <v>0.89755291005290905</v>
       </c>
       <c r="D17" s="4">
-        <v>5.18176221847534</v>
+        <v>45.323498725891099</v>
       </c>
       <c r="E17" s="10">
-        <v>0.81398999999999999</v>
+        <v>0.80125000000000002</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" s="4">
-        <v>0.91309523809523796</v>
+        <v>0.88029100529100501</v>
       </c>
       <c r="D18" s="4">
-        <v>45.2369995117187</v>
+        <v>6.1019423007964999</v>
       </c>
       <c r="E18" s="10">
-        <v>0.81652999999999998</v>
+        <v>0.77829999999999999</v>
       </c>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4">
-        <v>0.89318783068783003</v>
+        <v>0.85899999999999999</v>
       </c>
       <c r="D19" s="4">
-        <v>6.8079984188079798</v>
-      </c>
-      <c r="E19" s="11">
-        <v>0.78535999999999995</v>
-      </c>
-      <c r="F19" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="7">
+        <v>2</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="D20" s="4">
+        <v>80.043800000000005</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="7">
+        <v>2</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.862896825396825</v>
+      </c>
+      <c r="D21" s="4">
+        <v>82.433997392654405</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.75097999999999998</v>
+      </c>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="7">
+        <v>2</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.8821</v>
+      </c>
+      <c r="D22" s="4">
+        <v>64.049199999999999</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.77070000000000005</v>
+      </c>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="7">
         <v>3</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B23" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.91111111111111098</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5.18176221847534</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.81398999999999999</v>
+      </c>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="7">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.91309523809523796</v>
+      </c>
+      <c r="D24" s="4">
+        <v>45.2369995117187</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.81652999999999998</v>
+      </c>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="7">
+        <v>3</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.89318783068783003</v>
+      </c>
+      <c r="D25" s="4">
+        <v>6.8079984188079798</v>
+      </c>
+      <c r="E25" s="11">
+        <v>0.78535999999999995</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="7">
+        <v>3</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.877</v>
+      </c>
+      <c r="D26" s="4">
+        <v>79</v>
+      </c>
+      <c r="E26" s="11">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="7">
+        <v>3</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="D27" s="4">
+        <v>79.087699999999998</v>
+      </c>
+      <c r="E27" s="11">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="7">
+        <v>3</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C28" s="4">
         <v>0.87559523809523798</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D28" s="4">
         <v>96.338500499725299</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E28" s="10">
         <v>0.75775999999999999</v>
       </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" ht="13.8" customHeight="1">
-      <c r="A21" s="7">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" ht="13.75" customHeight="1">
+      <c r="A29" s="7">
         <v>3</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B29" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C29" s="4">
         <v>0.89670000000000005</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D29" s="4">
         <v>72.608500000000006</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E29" s="10">
         <v>0.78551000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated xlsx model results after tuning lgbm model
</commit_message>
<xml_diff>
--- a/2021_04_11_Final/model_results.xlsx
+++ b/2021_04_11_Final/model_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blairjones/Dropbox/-GradSchool/BerkeleyProgram/Semester2/W207-MachineLearning/w207_final_project_bwp/2021_04_11_Final/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinpi\MIDS\w207_final_project_bwp\2021_04_11_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609B029E-3D72-6442-8A7F-D63CA7FD6FDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869BA814-D10E-4464-88B9-D1CCB7A13FEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="1260" windowWidth="23140" windowHeight="13400" xr2:uid="{8502571B-A512-41BA-B560-0A8CC948E526}"/>
+    <workbookView xWindow="7068" yWindow="2064" windowWidth="15516" windowHeight="9882" xr2:uid="{8502571B-A512-41BA-B560-0A8CC948E526}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -594,16 +594,16 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="9.68359375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="20.83984375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="15.83984375" customWidth="1"/>
+    <col min="4" max="4" width="18.83984375" customWidth="1"/>
+    <col min="5" max="5" width="15.47265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -744,13 +744,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="4">
-        <v>0.87239999999999995</v>
+        <v>0.85929999999999995</v>
       </c>
       <c r="D8" s="4">
-        <v>56.443899999999999</v>
+        <v>47.740900000000003</v>
       </c>
       <c r="E8" s="10">
-        <v>0.75253999999999999</v>
+        <v>0.73341999999999996</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -870,13 +870,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="4">
-        <v>0.88090000000000002</v>
+        <v>0.872</v>
       </c>
       <c r="D15" s="4">
-        <v>64.006299999999996</v>
+        <v>54.332000000000001</v>
       </c>
       <c r="E15" s="10">
-        <v>0.76978000000000002</v>
+        <v>0.75524000000000002</v>
       </c>
       <c r="F15" s="2"/>
     </row>
@@ -996,13 +996,13 @@
         <v>9</v>
       </c>
       <c r="C22" s="4">
-        <v>0.8821</v>
+        <v>0.87480000000000002</v>
       </c>
       <c r="D22" s="4">
-        <v>64.049199999999999</v>
+        <v>55.395299999999999</v>
       </c>
       <c r="E22" s="10">
-        <v>0.77070000000000005</v>
+        <v>0.75480000000000003</v>
       </c>
       <c r="F22" s="2"/>
     </row>
@@ -1122,13 +1122,13 @@
         <v>9</v>
       </c>
       <c r="C29" s="4">
-        <v>0.89670000000000005</v>
+        <v>0.88580000000000003</v>
       </c>
       <c r="D29" s="4">
-        <v>72.608500000000006</v>
+        <v>60.159399999999998</v>
       </c>
       <c r="E29" s="10">
-        <v>0.78551000000000004</v>
+        <v>0.77078999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>